<commit_message>
read data fron excel sheet and pass to method
</commit_message>
<xml_diff>
--- a/wcsm9automationproject/src/main/resources/ActiTimeTestData.xlsx
+++ b/wcsm9automationproject/src/main/resources/ActiTimeTestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chinm\git\Wcsm9AutomationTesting\wcsm9automationproject\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9924618D-B129-4752-87EF-9654D10B5800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262BEC74-F57A-4051-A06A-C9AC4D8A701E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14169" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="validcreads" sheetId="1" r:id="rId1"/>
-    <sheet name="invalidcreads" sheetId="2" r:id="rId2"/>
+    <sheet name="validcreds" sheetId="1" r:id="rId1"/>
+    <sheet name="invalidcreds" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -126,13 +126,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,8 +414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -446,8 +445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2772AB17-CB6C-49A9-8905-2DF20CEB7B0D}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B8"/>
+    <sheetView zoomScale="142" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -489,26 +488,26 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>